<commit_message>
Test tape sensors, writing bumper sensors
</commit_message>
<xml_diff>
--- a/Schematics/Uno32_IO_board.xlsx
+++ b/Schematics/Uno32_IO_board.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14895"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="240">
   <si>
     <r>
       <rPr>
@@ -2069,15 +2069,9 @@
     <t>Hbridge Dir A</t>
   </si>
   <si>
-    <t>Hbrige Step A (PWM3)</t>
-  </si>
-  <si>
     <t>Hbridge Step A (PWM3)</t>
   </si>
   <si>
-    <t>Hbridge Dir B</t>
-  </si>
-  <si>
     <t>Gate  (RC Servo)</t>
   </si>
   <si>
@@ -2103,13 +2097,31 @@
   </si>
   <si>
     <t>TAPE_ARMRIGHT</t>
+  </si>
+  <si>
+    <t>Hbrige Dir B</t>
+  </si>
+  <si>
+    <t>Hbrige Step B (PWM2)</t>
+  </si>
+  <si>
+    <t>TAPE_LEDS1</t>
+  </si>
+  <si>
+    <t>TAPE_LEDS2</t>
+  </si>
+  <si>
+    <t>TAPE_LEDS3</t>
+  </si>
+  <si>
+    <t>TAPE_LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2465,6 +2477,66 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2478,7 +2550,25 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2486,37 +2576,43 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2524,90 +2620,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2910,14 +2922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44:K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="2" max="2" width="1.83203125" customWidth="1"/>
@@ -2929,919 +2941,919 @@
     <col min="8" max="8" width="41.33203125" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
     <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="1.33203125" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" customWidth="1"/>
     <col min="12" max="12" width="7.83203125" customWidth="1"/>
     <col min="13" max="13" width="73.33203125" customWidth="1"/>
     <col min="14" max="14" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20" customHeight="1">
+    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="47"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="45"/>
-    </row>
-    <row r="3" spans="1:12" ht="19" customHeight="1">
-      <c r="A3" s="49" t="s">
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" ht="18.95" customHeight="1">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="49" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="55"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="23"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="26"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="14"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="K5" s="57"/>
+      <c r="J5" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="K5" s="37"/>
       <c r="L5" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="23"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="K6" s="28"/>
+      <c r="J6" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="K6" s="39"/>
       <c r="L6" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="14"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="K7" s="19"/>
+      <c r="J7" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="K7" s="41"/>
       <c r="L7" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="K8" s="28"/>
+      <c r="J8" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" s="39"/>
       <c r="L8" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="14"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="K9" s="19"/>
+      <c r="J9" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="K9" s="41"/>
       <c r="L9" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="22" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="23"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="K10" s="28"/>
+      <c r="J10" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="K10" s="39"/>
       <c r="L10" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="34"/>
+      <c r="E11" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="14"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="K11" s="19"/>
+      <c r="J11" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="K11" s="41"/>
       <c r="L11" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="22" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="23"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="K12" s="28"/>
+      <c r="J12" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="K12" s="39"/>
       <c r="L12" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="34"/>
+      <c r="E13" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="14"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="58" t="s">
+      <c r="J13" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="K13" s="43"/>
+      <c r="L13" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="22" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="23"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="26"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="34"/>
+      <c r="E15" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="14"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="17"/>
+      <c r="K15" s="43"/>
       <c r="L15" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="21"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="K16" s="26"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="34"/>
+      <c r="E17" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="17"/>
+      <c r="K17" s="43"/>
       <c r="L17" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="25"/>
+      <c r="C18" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="20" t="s">
+      <c r="D18" s="27"/>
+      <c r="E18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="21"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="26"/>
+      <c r="K18" s="30"/>
       <c r="L18" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="34"/>
+      <c r="E19" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="12"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="32"/>
       <c r="H19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="17"/>
+      <c r="K19" s="43"/>
       <c r="L19" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="40" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="47"/>
+      <c r="E20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="26"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="34"/>
+      <c r="E21" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="12"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="43"/>
       <c r="L21" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="40" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="47"/>
+      <c r="E22" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="21"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="4" t="s">
         <v>109</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="K22" s="26"/>
+      <c r="K22" s="30"/>
       <c r="L22" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="34"/>
+      <c r="E23" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="5" t="s">
         <v>115</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="43"/>
       <c r="L23" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="20" t="s">
+      <c r="D24" s="27"/>
+      <c r="E24" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="21"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="4" t="s">
         <v>121</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="K24" s="26"/>
+      <c r="K24" s="30"/>
       <c r="L24" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="11" t="s">
+      <c r="D25" s="34"/>
+      <c r="E25" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="12"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="32"/>
       <c r="H25" s="5" t="s">
         <v>127</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="17"/>
+      <c r="K25" s="43"/>
       <c r="L25" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="27"/>
+      <c r="E26" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="21"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="4" t="s">
         <v>132</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="26"/>
+      <c r="K26" s="30"/>
       <c r="L26" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="11" t="s">
+      <c r="D27" s="34"/>
+      <c r="E27" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="12"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="5" t="s">
         <v>138</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="J27" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="K27" s="17"/>
+      <c r="K27" s="43"/>
       <c r="L27" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22" t="s">
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="20" t="s">
+      <c r="D28" s="27"/>
+      <c r="E28" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="21"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="4" t="s">
         <v>144</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="K28" s="26"/>
+      <c r="K28" s="30"/>
       <c r="L28" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35" t="s">
+      <c r="B29" s="49"/>
+      <c r="C29" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="33" t="s">
+      <c r="D29" s="51"/>
+      <c r="E29" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="49"/>
       <c r="H29" s="6" t="s">
         <v>150</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="J29" s="38" t="s">
+      <c r="J29" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="39"/>
+      <c r="K29" s="54"/>
       <c r="L29" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="20" t="s">
+      <c r="D30" s="27"/>
+      <c r="E30" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="21"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="4" t="s">
         <v>155</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J30" s="25" t="s">
+      <c r="J30" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="26"/>
+      <c r="K30" s="30"/>
       <c r="L30" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="34"/>
+      <c r="E31" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="12"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="32"/>
       <c r="H31" s="5" t="s">
         <v>160</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="43"/>
       <c r="L31" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="20" t="s">
+      <c r="D32" s="27"/>
+      <c r="E32" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="21"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="25"/>
       <c r="H32" s="4" t="s">
         <v>164</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J32" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="K32" s="32"/>
+      <c r="J32" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="K32" s="56"/>
       <c r="L32" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="11" t="s">
+      <c r="D33" s="34"/>
+      <c r="E33" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="12"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="32"/>
       <c r="H33" s="5" t="s">
         <v>168</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="J33" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="K33" s="30"/>
+      <c r="J33" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="K33" s="58"/>
       <c r="L33" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="20" t="s">
+      <c r="D34" s="27"/>
+      <c r="E34" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="21"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="25"/>
       <c r="H34" s="4" t="s">
         <v>172</v>
       </c>
@@ -3849,7 +3861,7 @@
         <v>173</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="8" t="s">
@@ -3857,462 +3869,315 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="32"/>
+      <c r="C35" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="11" t="s">
+      <c r="D35" s="34"/>
+      <c r="E35" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="12"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="32"/>
       <c r="H35" s="5" t="s">
         <v>176</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="J35" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="K35" s="32"/>
+      <c r="J35" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="K35" s="56"/>
       <c r="L35" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="20" t="s">
+      <c r="D36" s="27"/>
+      <c r="E36" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="21"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="4" t="s">
         <v>180</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="J36" s="29" t="s">
+      <c r="J36" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="K36" s="30"/>
+      <c r="K36" s="58"/>
       <c r="L36" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="11" t="s">
+      <c r="D37" s="34"/>
+      <c r="E37" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="12"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="32"/>
       <c r="H37" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="31" t="s">
+      <c r="J37" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="K37" s="32"/>
+      <c r="K37" s="56"/>
       <c r="L37" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22" t="s">
+      <c r="B38" s="25"/>
+      <c r="C38" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="20" t="s">
+      <c r="D38" s="27"/>
+      <c r="E38" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="21"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="4" t="s">
         <v>188</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J38" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="K38" s="30"/>
+      <c r="K38" s="58"/>
       <c r="L38" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13" t="s">
+      <c r="B39" s="32"/>
+      <c r="C39" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="11" t="s">
+      <c r="D39" s="34"/>
+      <c r="E39" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="12"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="32"/>
       <c r="H39" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J39" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="K39" s="17"/>
+      <c r="K39" s="43"/>
       <c r="L39" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="22" customHeight="1">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:12" ht="21.95" customHeight="1">
+      <c r="A40" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="25"/>
+      <c r="C40" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="20" t="s">
+      <c r="D40" s="27"/>
+      <c r="E40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="21"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="4" t="s">
         <v>197</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J40" s="27"/>
-      <c r="K40" s="28"/>
+      <c r="J40" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K40" s="39"/>
       <c r="L40" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="32"/>
+      <c r="C41" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="11" t="s">
+      <c r="D41" s="34"/>
+      <c r="E41" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="12"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="32"/>
       <c r="H41" s="5" t="s">
         <v>200</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="K41" s="17"/>
+      <c r="K41" s="43"/>
       <c r="L41" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="20" t="s">
+      <c r="D42" s="27"/>
+      <c r="E42" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="21"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="25"/>
       <c r="H42" s="4" t="s">
         <v>204</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J42" s="25" t="s">
+      <c r="J42" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K42" s="26"/>
+      <c r="K42" s="30"/>
       <c r="L42" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="20" customHeight="1">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="13" t="s">
+      <c r="B43" s="32"/>
+      <c r="C43" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="11" t="s">
+      <c r="D43" s="34"/>
+      <c r="E43" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="12"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="32"/>
       <c r="H43" s="5" t="s">
         <v>207</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="J43" s="18"/>
-      <c r="K43" s="19"/>
+      <c r="J43" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="K43" s="41"/>
       <c r="L43" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="24" customHeight="1">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="20" t="s">
+      <c r="D44" s="27"/>
+      <c r="E44" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="21"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="4" t="s">
         <v>212</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J44" s="27"/>
-      <c r="K44" s="28"/>
+      <c r="J44" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="K44" s="39"/>
       <c r="L44" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="13" t="s">
+      <c r="B45" s="32"/>
+      <c r="C45" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="11" t="s">
+      <c r="D45" s="34"/>
+      <c r="E45" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="12"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="32"/>
       <c r="H45" s="5" t="s">
         <v>216</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J45" s="18"/>
-      <c r="K45" s="19"/>
+      <c r="J45" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="K45" s="41"/>
       <c r="L45" s="8" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="175">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="J40:K40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:G41"/>
@@ -4333,6 +4198,161 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="J44:K44"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Finished IR code, updated tape test harness
</commit_message>
<xml_diff>
--- a/Schematics/Uno32_IO_board.xlsx
+++ b/Schematics/Uno32_IO_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="250">
   <si>
     <r>
       <rPr>
@@ -2075,9 +2075,6 @@
     <t>Gate  (RC Servo)</t>
   </si>
   <si>
-    <t>TAPE_LEDS</t>
-  </si>
-  <si>
     <t>TAPE_LEFT</t>
   </si>
   <si>
@@ -2115,13 +2112,46 @@
   </si>
   <si>
     <t>TAPE_LED</t>
+  </si>
+  <si>
+    <t>J1-11</t>
+  </si>
+  <si>
+    <t>J1-12</t>
+  </si>
+  <si>
+    <t>J1-7</t>
+  </si>
+  <si>
+    <t>J1-8</t>
+  </si>
+  <si>
+    <t>Hbridge</t>
+  </si>
+  <si>
+    <t>Perfboard</t>
+  </si>
+  <si>
+    <t>ULN G</t>
+  </si>
+  <si>
+    <t>ULN F</t>
+  </si>
+  <si>
+    <t>ULN E</t>
+  </si>
+  <si>
+    <t>ULN D</t>
+  </si>
+  <si>
+    <t>RC Servo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2187,8 +2217,43 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2222,8 +2287,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -2431,6 +2532,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2443,7 +2555,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2477,149 +2589,215 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2636,6 +2814,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>853439</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="gy.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6484620" y="1935481"/>
+          <a:ext cx="853439" cy="205739"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2923,10 +3144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44:K44"/>
+    <sheetView tabSelected="1" topLeftCell="I22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
@@ -2943,1238 +3164,1341 @@
     <col min="10" max="10" width="17.83203125" customWidth="1"/>
     <col min="11" max="11" width="2.83203125" customWidth="1"/>
     <col min="12" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="13" width="73.33203125" customWidth="1"/>
-    <col min="14" max="14" width="1.5" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="15" customWidth="1"/>
+    <col min="14" max="14" width="73.33203125" customWidth="1"/>
+    <col min="15" max="15" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:14" ht="24" customHeight="1">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="1:12" ht="18.95" customHeight="1">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:14" ht="18.95" customHeight="1">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="23"/>
+      <c r="K3" s="37"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:14" ht="15" customHeight="1">
+      <c r="A4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="41"/>
+      <c r="E4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="27"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="44"/>
       <c r="L4" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:14" ht="15" customHeight="1">
+      <c r="A5" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="34"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M5" s="16"/>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:14" ht="15" customHeight="1">
+      <c r="A6" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="26" t="s">
+      <c r="D6" s="41"/>
+      <c r="E6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="K6" s="39"/>
+      <c r="J6" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="K6" s="53"/>
       <c r="L6" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M6" s="18"/>
+      <c r="N6" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:14" ht="15" customHeight="1">
+      <c r="A7" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="33" t="s">
+      <c r="D7" s="48"/>
+      <c r="E7" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="34"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="K7" s="41"/>
+      <c r="J7" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="K7" s="55"/>
       <c r="L7" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M7" s="21"/>
+      <c r="N7" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:14" ht="15" customHeight="1">
+      <c r="A8" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="26" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="K8" s="39"/>
+      <c r="J8" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="K8" s="53"/>
       <c r="L8" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M8" s="24"/>
+      <c r="N8" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:14" ht="15" customHeight="1">
+      <c r="A9" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="33" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="34"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="K9" s="41"/>
+      <c r="J9" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="K9" s="55"/>
       <c r="L9" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M9" s="23"/>
+      <c r="N9" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:14" ht="15" customHeight="1">
+      <c r="A10" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="26" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="27"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="K10" s="39"/>
+      <c r="J10" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="K10" s="53"/>
       <c r="L10" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M10" s="16"/>
+      <c r="N10" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:14" ht="15" customHeight="1">
+      <c r="A11" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="46"/>
+      <c r="C11" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33" t="s">
+      <c r="D11" s="48"/>
+      <c r="E11" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="34"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="40" t="s">
-        <v>232</v>
-      </c>
-      <c r="K11" s="41"/>
+      <c r="J11" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="K11" s="55"/>
       <c r="L11" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M11" s="25"/>
+      <c r="N11" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1">
-      <c r="A12" s="24" t="s">
+    <row r="12" spans="1:14" ht="15" customHeight="1">
+      <c r="A12" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="K12" s="39"/>
+      <c r="J12" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="K12" s="53"/>
       <c r="L12" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M12" s="20"/>
+      <c r="N12" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:14" ht="15" customHeight="1">
+      <c r="A13" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33" t="s">
+      <c r="B13" s="46"/>
+      <c r="C13" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="33" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="42" t="s">
-        <v>226</v>
-      </c>
-      <c r="K13" s="43"/>
-      <c r="L13" s="11" t="s">
+      <c r="J13" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="K13" s="57"/>
+      <c r="L13" s="78" t="s">
         <v>218</v>
       </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="80" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="24" t="s">
+    <row r="14" spans="1:14" ht="15" customHeight="1">
+      <c r="A14" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="27"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="44"/>
       <c r="L14" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M14" s="16"/>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="31" t="s">
+    <row r="15" spans="1:14" ht="15" customHeight="1">
+      <c r="A15" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="46"/>
+      <c r="C15" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="33" t="s">
+      <c r="D15" s="48"/>
+      <c r="E15" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="34"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="43"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="7" t="s">
         <v>218</v>
       </c>
+      <c r="M15" s="16"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="24" t="s">
+    <row r="16" spans="1:14" ht="15" customHeight="1">
+      <c r="A16" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="24" t="s">
+      <c r="D16" s="41"/>
+      <c r="E16" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="25"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="K16" s="30"/>
+      <c r="K16" s="44"/>
       <c r="L16" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M16" s="16"/>
     </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="31" t="s">
+    <row r="17" spans="1:14" ht="15" customHeight="1">
+      <c r="A17" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33" t="s">
+      <c r="B17" s="46"/>
+      <c r="C17" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="31" t="s">
+      <c r="D17" s="48"/>
+      <c r="E17" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="32"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="43"/>
+      <c r="K17" s="57"/>
       <c r="L17" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M17" s="16"/>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:14" ht="15" customHeight="1">
+      <c r="A18" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="24" t="s">
+      <c r="D18" s="41"/>
+      <c r="E18" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="25"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="30"/>
+      <c r="K18" s="44"/>
       <c r="L18" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M18" s="16"/>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
-      <c r="A19" s="31" t="s">
+    <row r="19" spans="1:14" ht="15" customHeight="1">
+      <c r="A19" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="31" t="s">
+      <c r="D19" s="48"/>
+      <c r="E19" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="32"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="43"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M19" s="16"/>
     </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:14" ht="18" customHeight="1">
+      <c r="A20" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="46" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="24" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="25"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="30"/>
+      <c r="K20" s="44"/>
       <c r="L20" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M20" s="16"/>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:14" ht="15" customHeight="1">
+      <c r="A21" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33" t="s">
+      <c r="B21" s="46"/>
+      <c r="C21" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="31" t="s">
+      <c r="D21" s="48"/>
+      <c r="E21" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="32"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="46"/>
       <c r="H21" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="43"/>
+      <c r="K21" s="57"/>
       <c r="L21" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M21" s="16"/>
     </row>
-    <row r="22" spans="1:12" ht="18" customHeight="1">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:14" ht="18" customHeight="1">
+      <c r="A22" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="46" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="24" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="25"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="4" t="s">
         <v>109</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="K22" s="30"/>
+      <c r="K22" s="44"/>
       <c r="L22" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M22" s="16"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:14" ht="15" customHeight="1">
+      <c r="A23" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33" t="s">
+      <c r="B23" s="46"/>
+      <c r="C23" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="31" t="s">
+      <c r="D23" s="48"/>
+      <c r="E23" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="32"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="46"/>
       <c r="H23" s="5" t="s">
         <v>115</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="K23" s="43"/>
+      <c r="K23" s="57"/>
       <c r="L23" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M23" s="16"/>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:14" ht="15" customHeight="1">
+      <c r="A24" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="24" t="s">
+      <c r="D24" s="41"/>
+      <c r="E24" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="25"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="4" t="s">
         <v>121</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="K24" s="30"/>
+      <c r="K24" s="44"/>
       <c r="L24" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:14" ht="15" customHeight="1">
+      <c r="A25" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33" t="s">
+      <c r="B25" s="46"/>
+      <c r="C25" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="31" t="s">
+      <c r="D25" s="48"/>
+      <c r="E25" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="46"/>
       <c r="H25" s="5" t="s">
         <v>127</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="43"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M25" s="16"/>
     </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="A26" s="24" t="s">
+    <row r="26" spans="1:14" ht="15" customHeight="1">
+      <c r="A26" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="39"/>
+      <c r="C26" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="24" t="s">
+      <c r="D26" s="41"/>
+      <c r="E26" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="44"/>
-      <c r="G26" s="25"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="4" t="s">
         <v>132</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="30"/>
+      <c r="K26" s="44"/>
       <c r="L26" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M26" s="16"/>
     </row>
-    <row r="27" spans="1:12" ht="18" customHeight="1">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:14" ht="18" customHeight="1">
+      <c r="A27" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33" t="s">
+      <c r="B27" s="46"/>
+      <c r="C27" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="31" t="s">
+      <c r="D27" s="48"/>
+      <c r="E27" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="G27" s="32"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="5" t="s">
         <v>138</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J27" s="42" t="s">
+      <c r="J27" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="K27" s="43"/>
+      <c r="K27" s="57"/>
       <c r="L27" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M27" s="16"/>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1">
-      <c r="A28" s="24" t="s">
+    <row r="28" spans="1:14" ht="15" customHeight="1">
+      <c r="A28" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="24" t="s">
+      <c r="D28" s="41"/>
+      <c r="E28" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="25"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="4" t="s">
         <v>144</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="K28" s="30"/>
+      <c r="K28" s="44"/>
       <c r="L28" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M28" s="16"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1">
-      <c r="A29" s="48" t="s">
+    <row r="29" spans="1:14" ht="15" customHeight="1">
+      <c r="A29" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50" t="s">
+      <c r="B29" s="63"/>
+      <c r="C29" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="48" t="s">
+      <c r="D29" s="65"/>
+      <c r="E29" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="49"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="63"/>
       <c r="H29" s="6" t="s">
         <v>150</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="J29" s="53" t="s">
+      <c r="J29" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="54"/>
+      <c r="K29" s="68"/>
       <c r="L29" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M29" s="16"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1">
-      <c r="A30" s="24" t="s">
+    <row r="30" spans="1:14" ht="15" customHeight="1">
+      <c r="A30" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="24" t="s">
+      <c r="D30" s="41"/>
+      <c r="E30" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="25"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="4" t="s">
         <v>155</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="30"/>
+      <c r="K30" s="44"/>
       <c r="L30" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1">
-      <c r="A31" s="31" t="s">
+    <row r="31" spans="1:14" ht="15" customHeight="1">
+      <c r="A31" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="33" t="s">
+      <c r="B31" s="46"/>
+      <c r="C31" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="31" t="s">
+      <c r="D31" s="48"/>
+      <c r="E31" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="32"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="5" t="s">
         <v>160</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="J31" s="42"/>
-      <c r="K31" s="43"/>
+      <c r="J31" s="75" t="s">
+        <v>235</v>
+      </c>
+      <c r="K31" s="57"/>
       <c r="L31" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M31" s="16"/>
+      <c r="N31" s="80" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1">
-      <c r="A32" s="24" t="s">
+    <row r="32" spans="1:14" ht="15" customHeight="1">
+      <c r="A32" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="39"/>
+      <c r="C32" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="24" t="s">
+      <c r="D32" s="41"/>
+      <c r="E32" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="25"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="39"/>
       <c r="H32" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="J32" s="55" t="s">
+      <c r="J32" s="69" t="s">
         <v>223</v>
       </c>
-      <c r="K32" s="56"/>
+      <c r="K32" s="70"/>
       <c r="L32" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M32" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="N32" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1">
-      <c r="A33" s="31" t="s">
+    <row r="33" spans="1:14" ht="15" customHeight="1">
+      <c r="A33" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="33" t="s">
+      <c r="B33" s="46"/>
+      <c r="C33" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="31" t="s">
+      <c r="D33" s="48"/>
+      <c r="E33" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="32"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="J33" s="57" t="s">
+      <c r="J33" s="71" t="s">
         <v>224</v>
       </c>
-      <c r="K33" s="58"/>
+      <c r="K33" s="72"/>
       <c r="L33" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M33" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="N33" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1">
-      <c r="A34" s="24" t="s">
+    <row r="34" spans="1:14" ht="15" customHeight="1">
+      <c r="A34" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="39"/>
+      <c r="C34" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="24" t="s">
+      <c r="D34" s="41"/>
+      <c r="E34" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="44"/>
-      <c r="G34" s="25"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="13" t="s">
         <v>173</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M34" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N34" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1">
-      <c r="A35" s="31" t="s">
+    <row r="35" spans="1:14" ht="15" customHeight="1">
+      <c r="A35" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="33" t="s">
+      <c r="B35" s="46"/>
+      <c r="C35" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="31" t="s">
+      <c r="D35" s="48"/>
+      <c r="E35" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="32"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="J35" s="55" t="s">
-        <v>235</v>
-      </c>
-      <c r="K35" s="56"/>
+      <c r="J35" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="K35" s="70"/>
       <c r="L35" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M35" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="N35" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:14" ht="15" customHeight="1">
+      <c r="A36" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="24" t="s">
+      <c r="D36" s="41"/>
+      <c r="E36" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="44"/>
-      <c r="G36" s="25"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="39"/>
       <c r="H36" s="4" t="s">
         <v>180</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="J36" s="57" t="s">
+      <c r="J36" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="K36" s="58"/>
+      <c r="K36" s="72"/>
       <c r="L36" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M36" s="23"/>
+      <c r="N36" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1">
-      <c r="A37" s="31" t="s">
+    <row r="37" spans="1:14" ht="15" customHeight="1">
+      <c r="A37" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33" t="s">
+      <c r="B37" s="46"/>
+      <c r="C37" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="31" t="s">
+      <c r="D37" s="48"/>
+      <c r="E37" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="32"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="55" t="s">
+      <c r="J37" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="K37" s="56"/>
+      <c r="K37" s="70"/>
       <c r="L37" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M37" s="22"/>
+      <c r="N37" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1">
-      <c r="A38" s="24" t="s">
+    <row r="38" spans="1:14" ht="15" customHeight="1">
+      <c r="A38" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="39"/>
+      <c r="C38" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="24" t="s">
+      <c r="D38" s="41"/>
+      <c r="E38" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="44"/>
-      <c r="G38" s="25"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="39"/>
       <c r="H38" s="4" t="s">
         <v>188</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J38" s="57" t="s">
+      <c r="J38" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="K38" s="58"/>
+      <c r="K38" s="72"/>
       <c r="L38" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M38" s="73"/>
+      <c r="N38" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1">
-      <c r="A39" s="31" t="s">
+    <row r="39" spans="1:14" ht="15" customHeight="1">
+      <c r="A39" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33" t="s">
+      <c r="B39" s="46"/>
+      <c r="C39" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="31" t="s">
+      <c r="D39" s="48"/>
+      <c r="E39" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="32"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="46"/>
       <c r="H39" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="J39" s="42" t="s">
+      <c r="J39" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="K39" s="43"/>
+      <c r="K39" s="57"/>
       <c r="L39" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M39" s="16"/>
     </row>
-    <row r="40" spans="1:12" ht="21.95" customHeight="1">
-      <c r="A40" s="24" t="s">
+    <row r="40" spans="1:14" ht="21.95" customHeight="1">
+      <c r="A40" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="39"/>
+      <c r="C40" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="41"/>
+      <c r="E40" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="25"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="39"/>
       <c r="H40" s="4" t="s">
         <v>197</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J40" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="K40" s="39"/>
+      <c r="J40" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="K40" s="53"/>
       <c r="L40" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M40" s="16"/>
+      <c r="N40" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1">
-      <c r="A41" s="31" t="s">
+    <row r="41" spans="1:14" ht="15" customHeight="1">
+      <c r="A41" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="33" t="s">
+      <c r="B41" s="46"/>
+      <c r="C41" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="31" t="s">
+      <c r="D41" s="48"/>
+      <c r="E41" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="32"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="5" t="s">
         <v>200</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="J41" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="K41" s="43"/>
+      <c r="J41" s="77" t="s">
+        <v>249</v>
+      </c>
+      <c r="K41" s="76"/>
       <c r="L41" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M41" s="16"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1">
-      <c r="A42" s="24" t="s">
+    <row r="42" spans="1:14" ht="15" customHeight="1">
+      <c r="A42" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26" t="s">
+      <c r="B42" s="39"/>
+      <c r="C42" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="24" t="s">
+      <c r="D42" s="41"/>
+      <c r="E42" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="25"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="4" t="s">
         <v>204</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J42" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="K42" s="30"/>
+      <c r="J42" s="79" t="s">
+        <v>249</v>
+      </c>
+      <c r="K42" s="53"/>
       <c r="L42" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M42" s="16"/>
     </row>
-    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="31" t="s">
+    <row r="43" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="33" t="s">
+      <c r="B43" s="46"/>
+      <c r="C43" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="31" t="s">
+      <c r="D43" s="48"/>
+      <c r="E43" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="G43" s="32"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="46"/>
       <c r="H43" s="5" t="s">
         <v>207</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="J43" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="K43" s="41"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="55"/>
       <c r="L43" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M43" s="16"/>
     </row>
-    <row r="44" spans="1:12" ht="24" customHeight="1">
-      <c r="A44" s="24" t="s">
+    <row r="44" spans="1:14" ht="24" customHeight="1">
+      <c r="A44" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="39"/>
+      <c r="C44" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="24" t="s">
+      <c r="D44" s="41"/>
+      <c r="E44" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="25"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="39"/>
       <c r="H44" s="4" t="s">
         <v>212</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J44" s="38" t="s">
+      <c r="J44" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="K44" s="39"/>
+      <c r="K44" s="53"/>
       <c r="L44" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M44" s="16"/>
+      <c r="N44" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="A45" s="31" t="s">
+    <row r="45" spans="1:14" ht="15" customHeight="1">
+      <c r="A45" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="33" t="s">
+      <c r="B45" s="46"/>
+      <c r="C45" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="31" t="s">
+      <c r="D45" s="48"/>
+      <c r="E45" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="32"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="46"/>
       <c r="H45" s="5" t="s">
         <v>216</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J45" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="K45" s="41"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="55"/>
       <c r="L45" s="8" t="s">
         <v>219</v>
       </c>
+      <c r="M45" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="175">
@@ -4355,7 +4679,8 @@
     <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Sunday, runs half of course.
</commit_message>
<xml_diff>
--- a/Schematics/Uno32_IO_board.xlsx
+++ b/Schematics/Uno32_IO_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="255">
   <si>
     <r>
       <rPr>
@@ -986,15 +986,6 @@
         <sz val="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>LED_BANK2_2*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>35</t>
     </r>
   </si>
@@ -1032,15 +1023,6 @@
         <rFont val="Arial"/>
       </rPr>
       <t>PORTX-08</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>LED_BANK2_3</t>
     </r>
   </si>
   <si>
@@ -1093,15 +1075,6 @@
         <sz val="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>LED_BANK2_0*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>55</t>
     </r>
   </si>
@@ -1147,15 +1120,6 @@
         <sz val="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>LED_BANK2_1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>52</t>
     </r>
   </si>
@@ -1201,15 +1165,6 @@
         <sz val="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PWM5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>54</t>
     </r>
   </si>
@@ -2105,9 +2060,6 @@
     <t>TAPE_LEDS1</t>
   </si>
   <si>
-    <t>TAPE_LEDS2</t>
-  </si>
-  <si>
     <t>TAPE_LEDS3</t>
   </si>
   <si>
@@ -2141,17 +2093,50 @@
     <t>ULN E</t>
   </si>
   <si>
-    <t>ULN D</t>
-  </si>
-  <si>
     <t>RC Servo</t>
+  </si>
+  <si>
+    <t>J2-D</t>
+  </si>
+  <si>
+    <t>ULN</t>
+  </si>
+  <si>
+    <t>DO NOT USE</t>
+  </si>
+  <si>
+    <t>LED_BANK2_1</t>
+  </si>
+  <si>
+    <t>LED_BANK2_2*, DNU</t>
+  </si>
+  <si>
+    <t>LED_BANK2_0*, DNU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR </t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>PWM5</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>LED_BANK2_3, TAPE_LEDS2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2252,8 +2237,24 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2320,6 +2321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2534,10 +2541,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -2555,7 +2562,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2607,9 +2614,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2634,6 +2638,30 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2724,6 +2752,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2742,6 +2776,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2763,6 +2812,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2775,29 +2827,17 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3146,8 +3186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
@@ -3175,1328 +3215,1352 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="24" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="29"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="27"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:14" ht="18.95" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="31" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="32"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="37"/>
+      <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="40" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="41"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="44"/>
+      <c r="K4" s="51"/>
       <c r="L4" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="48"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="50" t="s">
-        <v>225</v>
-      </c>
-      <c r="K5" s="51"/>
+      <c r="J5" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="K5" s="58"/>
       <c r="L5" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="48"/>
+      <c r="E6" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="41"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="K6" s="53"/>
+      <c r="J6" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="K6" s="60"/>
       <c r="L6" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M6" s="18"/>
+        <v>213</v>
+      </c>
+      <c r="M6" s="17"/>
       <c r="N6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="48"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="K7" s="55"/>
+      <c r="J7" s="61" t="s">
+        <v>222</v>
+      </c>
+      <c r="K7" s="62"/>
       <c r="L7" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M7" s="21"/>
+        <v>213</v>
+      </c>
+      <c r="M7" s="20"/>
       <c r="N7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40" t="s">
+      <c r="B8" s="46"/>
+      <c r="C8" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="40" t="s">
+      <c r="D8" s="48"/>
+      <c r="E8" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="41"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="52" t="s">
-        <v>228</v>
-      </c>
-      <c r="K8" s="53"/>
+      <c r="J8" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" s="60"/>
       <c r="L8" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M8" s="24"/>
+        <v>213</v>
+      </c>
+      <c r="M8" s="23"/>
       <c r="N8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="47" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="48"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="K9" s="55"/>
+      <c r="J9" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="K9" s="62"/>
       <c r="L9" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M9" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="M9" s="22"/>
       <c r="N9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="40" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="41"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="52" t="s">
-        <v>230</v>
-      </c>
-      <c r="K10" s="53"/>
+      <c r="J10" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="K10" s="60"/>
       <c r="L10" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M10" s="16"/>
       <c r="N10" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47" t="s">
+      <c r="B11" s="53"/>
+      <c r="C11" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="47" t="s">
+      <c r="D11" s="55"/>
+      <c r="E11" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="48"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="K11" s="55"/>
+      <c r="J11" s="61" t="s">
+        <v>226</v>
+      </c>
+      <c r="K11" s="62"/>
       <c r="L11" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M11" s="25"/>
+        <v>213</v>
+      </c>
+      <c r="M11" s="24"/>
       <c r="N11" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="40" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="41"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="53"/>
+      <c r="J12" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="K12" s="60"/>
       <c r="L12" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M12" s="20"/>
+        <v>213</v>
+      </c>
+      <c r="M12" s="19"/>
       <c r="N12" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47" t="s">
+      <c r="B13" s="53"/>
+      <c r="C13" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="47" t="s">
+      <c r="D13" s="55"/>
+      <c r="E13" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="48"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="75" t="s">
-        <v>236</v>
-      </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="78" t="s">
-        <v>218</v>
-      </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="80" t="s">
-        <v>248</v>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="M13" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="40" t="s">
+      <c r="D14" s="48"/>
+      <c r="E14" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="41"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="48"/>
       <c r="H14" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="43" t="s">
+      <c r="J14" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="44"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M14" s="16"/>
+        <v>213</v>
+      </c>
+      <c r="M14" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="N14" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47" t="s">
+      <c r="B15" s="53"/>
+      <c r="C15" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="47" t="s">
+      <c r="D15" s="55"/>
+      <c r="E15" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="49"/>
-      <c r="G15" s="48"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="57"/>
+      <c r="K15" s="66"/>
       <c r="L15" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="38" t="s">
+      <c r="D16" s="48"/>
+      <c r="E16" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="39"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="K16" s="44"/>
+      <c r="K16" s="51"/>
       <c r="L16" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M16" s="16"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="45" t="s">
+      <c r="D17" s="55"/>
+      <c r="E17" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="59"/>
-      <c r="G17" s="46"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="53"/>
       <c r="H17" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="56" t="s">
+      <c r="J17" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="57"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40" t="s">
+      <c r="B18" s="46"/>
+      <c r="C18" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="38" t="s">
+      <c r="D18" s="48"/>
+      <c r="E18" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="58"/>
-      <c r="G18" s="39"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="43" t="s">
+      <c r="J18" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="44"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="47" t="s">
+      <c r="B19" s="53"/>
+      <c r="C19" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="45" t="s">
+      <c r="D19" s="55"/>
+      <c r="E19" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="59"/>
-      <c r="G19" s="46"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="56" t="s">
+      <c r="J19" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="57"/>
+      <c r="K19" s="66"/>
       <c r="L19" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:14" ht="18" customHeight="1">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="60" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="38" t="s">
+      <c r="D20" s="70"/>
+      <c r="E20" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="58"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="44"/>
+      <c r="J20" s="71" t="s">
+        <v>247</v>
+      </c>
+      <c r="K20" s="72"/>
       <c r="L20" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M20" s="16"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1">
-      <c r="A21" s="45" t="s">
+    <row r="21" spans="1:14" ht="23.25" customHeight="1">
+      <c r="A21" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="47" t="s">
+      <c r="D21" s="55"/>
+      <c r="E21" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="45" t="s">
+      <c r="F21" s="68"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="59"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="K21" s="57"/>
+      <c r="J21" s="61" t="s">
+        <v>254</v>
+      </c>
+      <c r="K21" s="62"/>
       <c r="L21" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M21" s="16"/>
+        <v>214</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="18" customHeight="1">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="46"/>
+      <c r="C22" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="60" t="s">
+      <c r="I22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="58"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J22" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="K22" s="44"/>
+      <c r="J22" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="K22" s="72"/>
       <c r="L22" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="55"/>
+      <c r="E23" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="68"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="47" t="s">
+      <c r="I23" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="59"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="K23" s="57"/>
+      <c r="J23" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="K23" s="74"/>
       <c r="L23" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M23" s="16"/>
+        <v>214</v>
+      </c>
+      <c r="M23" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="N23" s="26" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="67"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="K24" s="44"/>
+      <c r="J24" s="75" t="s">
+        <v>251</v>
+      </c>
+      <c r="K24" s="51"/>
       <c r="L24" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M24" s="16"/>
+        <v>214</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="N24" s="26" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="68"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="59"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J25" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="K25" s="57"/>
+      <c r="K25" s="66"/>
       <c r="L25" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1">
-      <c r="A26" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="58"/>
-      <c r="G26" s="39"/>
+      <c r="A26" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="67"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J26" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="K26" s="44"/>
+        <v>128</v>
+      </c>
+      <c r="J26" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="K26" s="51"/>
       <c r="L26" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M26" s="16"/>
     </row>
     <row r="27" spans="1:14" ht="18" customHeight="1">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="53"/>
+      <c r="C27" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="55"/>
+      <c r="E27" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="68"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="J27" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="K27" s="57"/>
+      <c r="K27" s="66"/>
       <c r="L27" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M27" s="16"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="67"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" s="58"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J28" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="K28" s="44"/>
+      <c r="K28" s="51"/>
       <c r="L28" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1">
-      <c r="A29" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64" t="s">
-        <v>148</v>
-      </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="62" t="s">
-        <v>149</v>
-      </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="63"/>
+      <c r="A29" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="77"/>
+      <c r="C29" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="79"/>
+      <c r="E29" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="80"/>
+      <c r="G29" s="77"/>
       <c r="H29" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="68"/>
+      <c r="K29" s="82"/>
       <c r="L29" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M29" s="16"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1">
-      <c r="A30" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="F30" s="58"/>
-      <c r="G30" s="39"/>
+      <c r="A30" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="67"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="J30" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="J30" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="44"/>
+      <c r="K30" s="51"/>
       <c r="L30" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M30" s="16"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1">
-      <c r="A31" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="F31" s="59"/>
-      <c r="G31" s="46"/>
+      <c r="A31" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="53"/>
+      <c r="C31" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="55"/>
+      <c r="E31" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="68"/>
+      <c r="G31" s="53"/>
       <c r="H31" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="J31" s="75" t="s">
-        <v>235</v>
-      </c>
-      <c r="K31" s="57"/>
+        <v>156</v>
+      </c>
+      <c r="J31" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="K31" s="66"/>
       <c r="L31" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="80" t="s">
-        <v>246</v>
+      <c r="N31" s="26" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1">
-      <c r="A32" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="38" t="s">
+      <c r="A32" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="58"/>
-      <c r="G32" s="39"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="J32" s="69" t="s">
-        <v>223</v>
-      </c>
-      <c r="K32" s="70"/>
+        <v>160</v>
+      </c>
+      <c r="J32" s="84" t="s">
+        <v>218</v>
+      </c>
+      <c r="K32" s="85"/>
       <c r="L32" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M32" s="18" t="s">
-        <v>239</v>
+        <v>214</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="N32" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1">
-      <c r="A33" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="F33" s="59"/>
-      <c r="G33" s="46"/>
+      <c r="A33" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="53"/>
+      <c r="C33" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="55"/>
+      <c r="E33" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="68"/>
+      <c r="G33" s="53"/>
       <c r="H33" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="J33" s="71" t="s">
-        <v>224</v>
-      </c>
-      <c r="K33" s="72"/>
+        <v>164</v>
+      </c>
+      <c r="J33" s="86" t="s">
+        <v>219</v>
+      </c>
+      <c r="K33" s="87"/>
       <c r="L33" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M33" s="19" t="s">
-        <v>240</v>
+        <v>214</v>
+      </c>
+      <c r="M33" s="18" t="s">
+        <v>234</v>
       </c>
       <c r="N33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1">
-      <c r="A34" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="38" t="s">
+      <c r="A34" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="58"/>
-      <c r="G34" s="39"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M34" s="20" t="s">
-        <v>241</v>
+        <v>214</v>
+      </c>
+      <c r="M34" s="19" t="s">
+        <v>235</v>
       </c>
       <c r="N34" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1">
-      <c r="A35" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="45" t="s">
+      <c r="A35" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="53"/>
+      <c r="C35" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="55"/>
+      <c r="E35" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="46"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J35" s="69" t="s">
-        <v>234</v>
-      </c>
-      <c r="K35" s="70"/>
+        <v>172</v>
+      </c>
+      <c r="J35" s="84" t="s">
+        <v>229</v>
+      </c>
+      <c r="K35" s="85"/>
       <c r="L35" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="N35" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1">
-      <c r="A36" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="38" t="s">
+      <c r="A36" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="46"/>
+      <c r="C36" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="39"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="J36" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="K36" s="72"/>
+        <v>176</v>
+      </c>
+      <c r="J36" s="86" t="s">
+        <v>216</v>
+      </c>
+      <c r="K36" s="87"/>
       <c r="L36" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M36" s="23"/>
+        <v>214</v>
+      </c>
+      <c r="M36" s="22"/>
       <c r="N36" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1">
-      <c r="A37" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="45" t="s">
+      <c r="A37" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="53"/>
+      <c r="C37" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="55"/>
+      <c r="E37" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="59"/>
-      <c r="G37" s="46"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="53"/>
       <c r="H37" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="J37" s="69" t="s">
-        <v>220</v>
-      </c>
-      <c r="K37" s="70"/>
+        <v>180</v>
+      </c>
+      <c r="J37" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="K37" s="85"/>
       <c r="L37" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M37" s="22"/>
+        <v>214</v>
+      </c>
+      <c r="M37" s="21"/>
       <c r="N37" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
-      <c r="A38" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="38" t="s">
+      <c r="A38" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="58"/>
-      <c r="G38" s="39"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="46"/>
       <c r="H38" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J38" s="71" t="s">
-        <v>222</v>
-      </c>
-      <c r="K38" s="72"/>
+        <v>184</v>
+      </c>
+      <c r="J38" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="K38" s="87"/>
       <c r="L38" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="M38" s="73"/>
+        <v>214</v>
+      </c>
+      <c r="M38" s="25"/>
       <c r="N38" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1">
-      <c r="A39" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="F39" s="59"/>
-      <c r="G39" s="46"/>
+      <c r="A39" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="53"/>
+      <c r="C39" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="55"/>
+      <c r="E39" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="68"/>
+      <c r="G39" s="53"/>
       <c r="H39" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="J39" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="K39" s="57"/>
+        <v>188</v>
+      </c>
+      <c r="J39" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="K39" s="66"/>
       <c r="L39" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M39" s="16"/>
     </row>
     <row r="40" spans="1:14" ht="21.95" customHeight="1">
-      <c r="A40" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="38" t="s">
+      <c r="A40" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="48"/>
+      <c r="E40" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="58"/>
-      <c r="G40" s="39"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="J40" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="K40" s="53"/>
+        <v>193</v>
+      </c>
+      <c r="J40" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="K40" s="60"/>
       <c r="L40" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M40" s="16"/>
       <c r="N40" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="F41" s="59"/>
-      <c r="G41" s="46"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="54" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="55"/>
+      <c r="E41" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="68"/>
+      <c r="G41" s="53"/>
       <c r="H41" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="J41" s="77" t="s">
-        <v>249</v>
-      </c>
-      <c r="K41" s="76"/>
+        <v>196</v>
+      </c>
+      <c r="J41" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="K41" s="88"/>
       <c r="L41" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M41" s="16"/>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
-      <c r="A42" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="38" t="s">
+      <c r="A42" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="46"/>
+      <c r="C42" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="58"/>
-      <c r="G42" s="39"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="J42" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="K42" s="53"/>
+        <v>200</v>
+      </c>
+      <c r="J42" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="K42" s="60"/>
       <c r="L42" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M42" s="16"/>
     </row>
     <row r="43" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="46"/>
-      <c r="C43" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="F43" s="59"/>
-      <c r="G43" s="46"/>
+      <c r="A43" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="53"/>
+      <c r="C43" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43" s="55"/>
+      <c r="E43" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="68"/>
+      <c r="G43" s="53"/>
       <c r="H43" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="J43" s="54"/>
-      <c r="K43" s="55"/>
+        <v>203</v>
+      </c>
+      <c r="J43" s="61" t="s">
+        <v>245</v>
+      </c>
+      <c r="K43" s="62"/>
       <c r="L43" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M43" s="16"/>
     </row>
     <row r="44" spans="1:14" ht="24" customHeight="1">
-      <c r="A44" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40" t="s">
-        <v>210</v>
-      </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="F44" s="58"/>
-      <c r="G44" s="39"/>
+      <c r="A44" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="48"/>
+      <c r="E44" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" s="67"/>
+      <c r="G44" s="46"/>
       <c r="H44" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="J44" s="74" t="s">
-        <v>237</v>
-      </c>
-      <c r="K44" s="53"/>
+        <v>208</v>
+      </c>
+      <c r="J44" s="90" t="s">
+        <v>231</v>
+      </c>
+      <c r="K44" s="60"/>
       <c r="L44" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M44" s="16"/>
       <c r="N44" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1">
-      <c r="A45" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="46"/>
-      <c r="C45" s="47" t="s">
+      <c r="A45" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="53"/>
+      <c r="C45" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D45" s="55"/>
+      <c r="E45" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="F45" s="68"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="J45" s="61" t="s">
+        <v>245</v>
+      </c>
+      <c r="K45" s="62"/>
+      <c r="L45" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="D45" s="48"/>
-      <c r="E45" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="F45" s="59"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J45" s="54"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="M45" s="16"/>
     </row>
@@ -4679,8 +4743,7 @@
     <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Project finished. Turned in report.
</commit_message>
<xml_diff>
--- a/Schematics/Uno32_IO_board.xlsx
+++ b/Schematics/Uno32_IO_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="255">
   <si>
     <r>
       <rPr>
@@ -2096,30 +2096,12 @@
     <t>LED_BANK2_0*, DNU</t>
   </si>
   <si>
-    <t xml:space="preserve">IR </t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
     <t>PWM5</t>
   </si>
   <si>
-    <t>Angle</t>
-  </si>
-  <si>
     <t>IR</t>
   </si>
   <si>
-    <t>LED_BANK2_3, TAPE_LEDS2</t>
-  </si>
-  <si>
-    <t>Amber LED</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
     <t>J2-11 (F)</t>
   </si>
   <si>
@@ -2132,14 +2114,29 @@
     <t>J2-9 (D)</t>
   </si>
   <si>
-    <t>`</t>
+    <t>Gate (RC Servo)</t>
+  </si>
+  <si>
+    <t>Hbridge Step B (PWM6)</t>
+  </si>
+  <si>
+    <t>IR Angle (RC Servo)</t>
+  </si>
+  <si>
+    <t>IR Main (RC Servo)</t>
+  </si>
+  <si>
+    <t>TAPE_LEDS2 (LED_BANK2_3)</t>
+  </si>
+  <si>
+    <t>Perfboard2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2197,11 +2194,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="6" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
     </font>
@@ -2210,12 +2202,6 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF800000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2253,11 +2239,36 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="7" tint="-0.249977111117893"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2311,12 +2322,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2330,12 +2335,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2571,7 +2570,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2605,18 +2604,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2635,41 +2622,95 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2684,12 +2725,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2698,49 +2739,37 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2764,37 +2793,31 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2803,50 +2826,44 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3195,8 +3212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:K31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
@@ -3213,7 +3230,7 @@
     <col min="10" max="10" width="17.83203125" customWidth="1"/>
     <col min="11" max="11" width="2.83203125" customWidth="1"/>
     <col min="12" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="11" customWidth="1"/>
     <col min="14" max="14" width="73.33203125" customWidth="1"/>
     <col min="15" max="15" width="1.5" customWidth="1"/>
   </cols>
@@ -3224,946 +3241,937 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="24" customHeight="1">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="81" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="82"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="79" t="s">
+      <c r="J2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="80"/>
+      <c r="K2" s="29"/>
     </row>
-    <row r="3" spans="1:14" ht="18.95" customHeight="1">
-      <c r="A3" s="84" t="s">
+    <row r="3" spans="1:14" ht="23.25" customHeight="1">
+      <c r="A3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="86" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="84" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="85"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="90"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="44" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="64" t="s">
+      <c r="J4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="65"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="50"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="77" t="s">
-        <v>255</v>
-      </c>
-      <c r="K5" s="78"/>
+      <c r="J5" s="80" t="s">
+        <v>249</v>
+      </c>
+      <c r="K5" s="81"/>
       <c r="L5" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="22" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="44" t="s">
+      <c r="D6" s="43"/>
+      <c r="E6" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="45"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="43"/>
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="K6" s="48"/>
+      <c r="K6" s="53"/>
       <c r="L6" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M6" s="17"/>
+      <c r="M6" s="13"/>
       <c r="N6" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="K7" s="41"/>
+      <c r="K7" s="55"/>
       <c r="L7" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M7" s="20"/>
+      <c r="M7" s="16"/>
       <c r="N7" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="44" t="s">
+      <c r="D8" s="43"/>
+      <c r="E8" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="45"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="43"/>
       <c r="H8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="K8" s="48"/>
+      <c r="K8" s="53"/>
       <c r="L8" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M8" s="23"/>
+      <c r="M8" s="19"/>
       <c r="N8" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="35" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="36"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="50"/>
       <c r="H9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="K9" s="41"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M9" s="22"/>
+      <c r="M9" s="18"/>
       <c r="N9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="41"/>
+      <c r="C10" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="44" t="s">
+      <c r="D10" s="43"/>
+      <c r="E10" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="45"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="K10" s="48"/>
+      <c r="K10" s="53"/>
       <c r="L10" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M10" s="16"/>
+      <c r="M10" s="12"/>
       <c r="N10" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35" t="s">
+      <c r="B11" s="48"/>
+      <c r="C11" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="50"/>
+      <c r="E11" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="K11" s="41"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M11" s="24"/>
+      <c r="M11" s="20"/>
       <c r="N11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="44" t="s">
+      <c r="D12" s="43"/>
+      <c r="E12" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="73"/>
-      <c r="G12" s="45"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="K12" s="48"/>
+      <c r="K12" s="53"/>
       <c r="L12" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M12" s="19"/>
+      <c r="M12" s="15"/>
       <c r="N12" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35" t="s">
+      <c r="B13" s="48"/>
+      <c r="C13" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="35" t="s">
+      <c r="D13" s="50"/>
+      <c r="E13" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="36"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="75"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="30" t="s">
+      <c r="J13" s="83" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" s="84"/>
+      <c r="L13" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="26"/>
+      <c r="N13" s="24" t="s">
         <v>244</v>
-      </c>
-      <c r="N13" s="29" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44" t="s">
+      <c r="B14" s="41"/>
+      <c r="C14" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="44" t="s">
+      <c r="D14" s="43"/>
+      <c r="E14" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="45"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="43"/>
       <c r="H14" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="65"/>
+      <c r="J14" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="K14" s="86"/>
       <c r="L14" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M14" s="32" t="s">
-        <v>246</v>
-      </c>
+      <c r="M14" s="27"/>
       <c r="N14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="35" t="s">
+      <c r="D15" s="50"/>
+      <c r="E15" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="36"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="53"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M15" s="16"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44" t="s">
+      <c r="B16" s="41"/>
+      <c r="C16" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="42" t="s">
+      <c r="D16" s="43"/>
+      <c r="E16" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="64" t="s">
+      <c r="J16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="K16" s="65"/>
+      <c r="K16" s="46"/>
       <c r="L16" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M16" s="16"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="33" t="s">
+      <c r="D17" s="50"/>
+      <c r="E17" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="34"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="48"/>
       <c r="H17" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="52" t="s">
+      <c r="J17" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="53"/>
+      <c r="K17" s="57"/>
       <c r="L17" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M17" s="16"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44" t="s">
+      <c r="B18" s="41"/>
+      <c r="C18" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="42" t="s">
+      <c r="D18" s="43"/>
+      <c r="E18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="64" t="s">
+      <c r="J18" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="65"/>
+      <c r="K18" s="46"/>
       <c r="L18" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M18" s="16"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="33" t="s">
+      <c r="D19" s="50"/>
+      <c r="E19" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="34"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J19" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="53"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M19" s="16"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:14" ht="18" customHeight="1">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="69" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="42" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="71" t="s">
+      <c r="J20" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="K20" s="72"/>
+      <c r="K20" s="63"/>
       <c r="L20" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M20" s="16"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:14" ht="23.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35" t="s">
+      <c r="B21" s="48"/>
+      <c r="C21" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="33" t="s">
+      <c r="D21" s="50"/>
+      <c r="E21" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="5" t="s">
         <v>103</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="K21" s="41"/>
+      <c r="J21" s="91" t="s">
+        <v>253</v>
+      </c>
+      <c r="K21" s="92"/>
       <c r="L21" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M21" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="N21" s="29" t="s">
+      <c r="M21" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="N21" s="24" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="18" customHeight="1">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="69" t="s">
+      <c r="B22" s="41"/>
+      <c r="C22" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="70"/>
-      <c r="E22" s="42" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="4" t="s">
         <v>107</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="71" t="s">
+      <c r="J22" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="K22" s="72"/>
+      <c r="K22" s="63"/>
       <c r="L22" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M22" s="16"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35" t="s">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="50"/>
+      <c r="E23" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="34"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="5" t="s">
         <v>112</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J23" s="38" t="s">
+      <c r="J23" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="K23" s="67"/>
+      <c r="K23" s="65"/>
       <c r="L23" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M23" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="N23" s="26" t="s">
-        <v>243</v>
-      </c>
+      <c r="M23" s="93"/>
+      <c r="N23" s="22"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="44" t="s">
+      <c r="B24" s="41"/>
+      <c r="C24" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="42" t="s">
+      <c r="D24" s="43"/>
+      <c r="E24" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="41"/>
       <c r="H24" s="4" t="s">
         <v>117</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J24" s="68" t="s">
-        <v>245</v>
-      </c>
-      <c r="K24" s="65"/>
+      <c r="J24" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="K24" s="46"/>
       <c r="L24" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M24" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="N24" s="26" t="s">
-        <v>243</v>
-      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="22"/>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="33" t="s">
+      <c r="D25" s="50"/>
+      <c r="E25" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="34"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="5" t="s">
         <v>122</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J25" s="52" t="s">
+      <c r="J25" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K25" s="53"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M25" s="16"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="41"/>
+      <c r="C26" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="42" t="s">
+      <c r="D26" s="43"/>
+      <c r="E26" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="41"/>
       <c r="H26" s="4" t="s">
         <v>127</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="J26" s="64" t="s">
+      <c r="J26" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="K26" s="65"/>
+      <c r="K26" s="46"/>
       <c r="L26" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M26" s="16"/>
+      <c r="M26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="18" customHeight="1">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35" t="s">
+      <c r="B27" s="48"/>
+      <c r="C27" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="50"/>
+      <c r="E27" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="34"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="5" t="s">
         <v>133</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="J27" s="52" t="s">
+      <c r="J27" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="K27" s="53"/>
+      <c r="K27" s="57"/>
       <c r="L27" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M27" s="16"/>
+      <c r="M27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="44" t="s">
+      <c r="B28" s="41"/>
+      <c r="C28" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="42" t="s">
+      <c r="D28" s="43"/>
+      <c r="E28" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="F28" s="46"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="4" t="s">
         <v>139</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J28" s="64" t="s">
+      <c r="J28" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="K28" s="65"/>
+      <c r="K28" s="46"/>
       <c r="L28" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M28" s="16"/>
+      <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="59" t="s">
+      <c r="B29" s="68"/>
+      <c r="C29" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="57" t="s">
+      <c r="D29" s="70"/>
+      <c r="E29" s="67" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="58"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="68"/>
       <c r="H29" s="6" t="s">
         <v>145</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J29" s="62" t="s">
+      <c r="J29" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="63"/>
+      <c r="K29" s="73"/>
       <c r="L29" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M29" s="91" t="s">
-        <v>249</v>
-      </c>
+      <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44" t="s">
+      <c r="B30" s="41"/>
+      <c r="C30" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="42" t="s">
+      <c r="D30" s="43"/>
+      <c r="E30" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="43"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="4" t="s">
         <v>150</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="J30" s="64" t="s">
+      <c r="J30" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="65"/>
+      <c r="K30" s="46"/>
       <c r="L30" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M30" s="16"/>
+      <c r="M30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35" t="s">
+      <c r="B31" s="48"/>
+      <c r="C31" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="33" t="s">
+      <c r="D31" s="50"/>
+      <c r="E31" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="34"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="48"/>
       <c r="H31" s="5" t="s">
         <v>155</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="J31" s="66" t="s">
+      <c r="J31" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="K31" s="53"/>
+      <c r="K31" s="92"/>
       <c r="L31" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M31" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="N31" s="26" t="s">
+      <c r="M31" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="N31" s="22" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="44" t="s">
+      <c r="B32" s="41"/>
+      <c r="C32" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="42" t="s">
+      <c r="D32" s="43"/>
+      <c r="E32" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="J32" s="55" t="s">
+      <c r="J32" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="K32" s="56"/>
+      <c r="K32" s="75"/>
       <c r="L32" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M32" s="17" t="s">
+      <c r="M32" s="13" t="s">
         <v>231</v>
       </c>
       <c r="N32" t="s">
@@ -4171,33 +4179,33 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="48"/>
+      <c r="C33" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="33" t="s">
+      <c r="D33" s="50"/>
+      <c r="E33" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="34"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="48"/>
       <c r="H33" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="J33" s="50" t="s">
+      <c r="J33" s="76" t="s">
         <v>219</v>
       </c>
-      <c r="K33" s="51"/>
+      <c r="K33" s="77"/>
       <c r="L33" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="18" t="s">
+      <c r="M33" s="14" t="s">
         <v>232</v>
       </c>
       <c r="N33" t="s">
@@ -4205,23 +4213,23 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="44" t="s">
+      <c r="B34" s="41"/>
+      <c r="C34" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="42" t="s">
+      <c r="D34" s="43"/>
+      <c r="E34" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="46"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="4" t="s">
         <v>168</v>
       </c>
       <c r="J34" s="9" t="s">
@@ -4231,7 +4239,7 @@
       <c r="L34" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="19" t="s">
+      <c r="M34" s="15" t="s">
         <v>233</v>
       </c>
       <c r="N34" t="s">
@@ -4239,33 +4247,33 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35" t="s">
+      <c r="B35" s="48"/>
+      <c r="C35" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="33" t="s">
+      <c r="D35" s="50"/>
+      <c r="E35" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="34"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="48"/>
       <c r="H35" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="J35" s="55" t="s">
+      <c r="J35" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="K35" s="56"/>
+      <c r="K35" s="75"/>
       <c r="L35" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="M35" s="12" t="s">
         <v>234</v>
       </c>
       <c r="N35" t="s">
@@ -4273,471 +4281,316 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44" t="s">
+      <c r="B36" s="41"/>
+      <c r="C36" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="42" t="s">
+      <c r="D36" s="43"/>
+      <c r="E36" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="4" t="s">
         <v>175</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="J36" s="50" t="s">
+      <c r="J36" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="K36" s="51"/>
+      <c r="K36" s="95"/>
       <c r="L36" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M36" s="22"/>
-      <c r="N36" t="s">
-        <v>236</v>
+      <c r="M36" s="18"/>
+      <c r="N36" s="22" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35" t="s">
+      <c r="B37" s="48"/>
+      <c r="C37" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="33" t="s">
+      <c r="D37" s="50"/>
+      <c r="E37" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="37"/>
-      <c r="G37" s="34"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="48"/>
       <c r="H37" s="5" t="s">
         <v>179</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J37" s="55" t="s">
+      <c r="J37" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="K37" s="56"/>
+      <c r="K37" s="97"/>
       <c r="L37" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M37" s="21"/>
-      <c r="N37" t="s">
-        <v>236</v>
+      <c r="M37" s="17"/>
+      <c r="N37" s="22" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44" t="s">
+      <c r="B38" s="41"/>
+      <c r="C38" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="42" t="s">
+      <c r="D38" s="43"/>
+      <c r="E38" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="46"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="41"/>
       <c r="H38" s="4" t="s">
         <v>183</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="J38" s="50" t="s">
+      <c r="J38" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="K38" s="51"/>
+      <c r="K38" s="95"/>
       <c r="L38" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M38" s="25"/>
-      <c r="N38" t="s">
-        <v>236</v>
+      <c r="M38" s="21"/>
+      <c r="N38" s="22" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="48"/>
+      <c r="C39" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="33" t="s">
+      <c r="D39" s="50"/>
+      <c r="E39" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="34"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="48"/>
       <c r="H39" s="5" t="s">
         <v>187</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="J39" s="52" t="s">
+      <c r="J39" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="K39" s="53"/>
+      <c r="K39" s="57"/>
       <c r="L39" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M39" s="16"/>
+      <c r="M39" s="12"/>
     </row>
     <row r="40" spans="1:14" ht="21.95" customHeight="1">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="44" t="s">
+      <c r="B40" s="41"/>
+      <c r="C40" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="42" t="s">
+      <c r="D40" s="43"/>
+      <c r="E40" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="46"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="41"/>
       <c r="H40" s="4" t="s">
         <v>192</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="J40" s="54" t="s">
+      <c r="J40" s="89" t="s">
         <v>230</v>
       </c>
-      <c r="K40" s="48"/>
+      <c r="K40" s="90"/>
       <c r="L40" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M40" s="16" t="s">
-        <v>252</v>
+      <c r="M40" s="12" t="s">
+        <v>246</v>
       </c>
       <c r="N40" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35" t="s">
+      <c r="B41" s="48"/>
+      <c r="C41" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="33" t="s">
+      <c r="D41" s="50"/>
+      <c r="E41" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="F41" s="37"/>
-      <c r="G41" s="34"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="48"/>
       <c r="H41" s="5" t="s">
         <v>195</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J41" s="38" t="s">
+      <c r="J41" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="K41" s="39"/>
+      <c r="K41" s="78"/>
       <c r="L41" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M41" s="16"/>
+      <c r="M41" s="12"/>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44" t="s">
+      <c r="B42" s="41"/>
+      <c r="C42" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="42" t="s">
+      <c r="D42" s="43"/>
+      <c r="E42" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="41"/>
       <c r="H42" s="4" t="s">
         <v>199</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J42" s="47" t="s">
+      <c r="J42" s="79" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="48"/>
+      <c r="K42" s="53"/>
       <c r="L42" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M42" s="16"/>
+      <c r="M42" s="12"/>
     </row>
     <row r="43" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35" t="s">
+      <c r="B43" s="48"/>
+      <c r="C43" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="D43" s="36"/>
-      <c r="E43" s="33" t="s">
+      <c r="D43" s="50"/>
+      <c r="E43" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="34"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="48"/>
       <c r="H43" s="5" t="s">
         <v>202</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="40" t="s">
+      <c r="J43" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="K43" s="41"/>
+      <c r="K43" s="88"/>
       <c r="L43" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="16"/>
+      <c r="M43" s="12"/>
     </row>
     <row r="44" spans="1:14" ht="24" customHeight="1">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="44" t="s">
+      <c r="B44" s="41"/>
+      <c r="C44" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="42" t="s">
+      <c r="D44" s="43"/>
+      <c r="E44" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="F44" s="46"/>
-      <c r="G44" s="43"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="41"/>
       <c r="H44" s="4" t="s">
         <v>207</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="J44" s="49" t="s">
+      <c r="J44" s="89" t="s">
         <v>229</v>
       </c>
-      <c r="K44" s="48"/>
+      <c r="K44" s="90"/>
       <c r="L44" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="16" t="s">
-        <v>253</v>
+      <c r="M44" s="12" t="s">
+        <v>247</v>
       </c>
       <c r="N44" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="35" t="s">
+      <c r="B45" s="48"/>
+      <c r="C45" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="33" t="s">
+      <c r="D45" s="50"/>
+      <c r="E45" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="34"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="48"/>
       <c r="H45" s="5" t="s">
         <v>211</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="J45" s="40" t="s">
+      <c r="J45" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="K45" s="41"/>
+      <c r="K45" s="88"/>
       <c r="L45" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="16"/>
+      <c r="M45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="175">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="J40:K40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:G41"/>
@@ -4758,6 +4611,161 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="J44:K44"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>